<commit_message>
fix zoneManagerDialog, referenceWindowDialog restructure wi-histogram
</commit_message>
<xml_diff>
--- a/Wi-Histogram.xlsx
+++ b/Wi-Histogram.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Github\wi-angular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/workspace/revoltech/wi-angular/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="HistogramTab" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
   <si>
     <t>Code</t>
   </si>
@@ -246,12 +249,21 @@
   </si>
   <si>
     <t>wiHistogram.histogramModel.properties.plotType=='Percent'</t>
+  </si>
+  <si>
+    <t>ZoneButton</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>wiHistogram.isShowWiZone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -639,24 +651,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -853,7 +865,7 @@
         <v>Button</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ref="F7:F36" si="3">SUBSTITUTE(E7,"_","-")</f>
+        <f t="shared" ref="F7:F37" si="3">SUBSTITUTE(E7,"_","-")</f>
         <v/>
       </c>
       <c r="G7" t="s">
@@ -891,7 +903,7 @@
         <v>2.1</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -905,7 +917,7 @@
         <v/>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="H9" t="s">
         <v>63</v>
@@ -914,35 +926,35 @@
         <v>12</v>
       </c>
       <c r="K9" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="M9" s="9">
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="10">
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="str">
-        <f>REPLACE(C10, 1, 2, "")</f>
+        <f t="shared" ref="D10" si="4">REPLACE(C10, 1, 2, "")</f>
         <v>Button</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F10" si="5">SUBSTITUTE(E10,"_","-")</f>
         <v/>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H10" t="s">
         <v>63</v>
@@ -951,21 +963,21 @@
         <v>12</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
-      </c>
-      <c r="M10">
+        <v>52</v>
+      </c>
+      <c r="M10" s="9">
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="6">
         <v>2.2999999999999998</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -979,7 +991,7 @@
         <v/>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H11" t="s">
         <v>63</v>
@@ -988,21 +1000,21 @@
         <v>12</v>
       </c>
       <c r="K11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="10">
         <v>2.4</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -1016,7 +1028,7 @@
         <v/>
       </c>
       <c r="G12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
         <v>63</v>
@@ -1025,120 +1037,120 @@
         <v>12</v>
       </c>
       <c r="K12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
       <c r="N12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="str">
+        <f>REPLACE(C13, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="1" t="str">
-        <f t="shared" ref="D13" si="4">REPLACE(C13, 1, 2, "")</f>
+      <c r="D14" s="1" t="str">
+        <f t="shared" ref="D14" si="6">REPLACE(C14, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="8" t="str">
-        <f t="shared" ref="D14:D28" si="5">REPLACE(C14, 1, 2, "")</f>
+      <c r="D15" s="8" t="str">
+        <f t="shared" ref="D15:D29" si="7">REPLACE(C15, 1, 2, "")</f>
         <v>Dropdown</v>
       </c>
-      <c r="F14" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="F15" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="5"/>
-        <v>Button</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" t="s">
-        <v>49</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
-        <v>72</v>
+      <c r="J15" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Button</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" ref="F16" si="6">SUBSTITUTE(E16,"_","-")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H16" t="s">
         <v>63</v>
@@ -1153,91 +1165,91 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="7"/>
+        <v>Button</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" ref="F17" si="8">SUBSTITUTE(E17,"_","-")</f>
+        <v/>
+      </c>
+      <c r="G17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="8" t="str">
-        <f t="shared" si="5"/>
+      <c r="D18" s="8" t="str">
+        <f t="shared" si="7"/>
         <v>Dropdown</v>
       </c>
-      <c r="F17" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="F18" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="5"/>
-        <v>Button</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" t="s">
-        <v>49</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
+      <c r="J18" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" ref="D19" si="7">REPLACE(C19, 1, 2, "")</f>
+        <f t="shared" si="7"/>
         <v>Button</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" ref="F19" si="8">SUBSTITUTE(E19,"_","-")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H19" t="s">
         <v>63</v>
@@ -1252,22 +1264,49 @@
         <v>1</v>
       </c>
       <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" ref="D20" si="9">REPLACE(C20, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" ref="F20" si="10">SUBSTITUTE(E20,"_","-")</f>
+        <v/>
+      </c>
+      <c r="G20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D20" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="N20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F21" t="str">
@@ -1277,7 +1316,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F22" t="str">
@@ -1287,7 +1326,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F23" t="str">
@@ -1297,7 +1336,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F24" t="str">
@@ -1307,7 +1346,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F25" t="str">
@@ -1317,7 +1356,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F26" t="str">
@@ -1327,7 +1366,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F27" t="str">
@@ -1337,7 +1376,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F28" t="str">
@@ -1347,7 +1386,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D29" t="str">
-        <f>REPLACE(C29, 1, 2, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F29" t="str">
@@ -1356,6 +1395,10 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D30" t="str">
+        <f>REPLACE(C30, 1, 2, "")</f>
+        <v/>
+      </c>
       <c r="F30" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1393,6 +1436,12 @@
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F36" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>

</xml_diff>